<commit_message>
wd removed from 2013 data
</commit_message>
<xml_diff>
--- a/_docs/Data cleaning scripts/ridership/November 2013.xlsx
+++ b/_docs/Data cleaning scripts/ridership/November 2013.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24526"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="480" windowWidth="15480" windowHeight="9720"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28280"/>
   </bookViews>
   <sheets>
     <sheet name="Weekday OD" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,17 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'Sunday OD'!$A:$A</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Weekday OD'!$A:$A</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="64">
   <si>
     <t>Exit stations</t>
   </si>
@@ -624,30 +629,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BE64"/>
+  <dimension ref="A1:BE63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="AX3" sqref="AX3"/>
       <selection pane="topRight" activeCell="AX3" sqref="AX3"/>
       <selection pane="bottomLeft" activeCell="AX3" sqref="AX3"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="A46" sqref="A46:XFD46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="45" width="7.7109375" style="9" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="8.7109375" style="11" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="9.140625" style="11" collapsed="1"/>
-    <col min="48" max="49" width="9.140625" style="9" collapsed="1"/>
-    <col min="50" max="50" width="8.7109375" style="9" customWidth="1" collapsed="1"/>
-    <col min="51" max="16384" width="9.140625" style="9" collapsed="1"/>
+    <col min="1" max="44" width="7.6640625" style="9" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="8.6640625" style="11" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="8.83203125" style="11" collapsed="1"/>
+    <col min="47" max="48" width="8.83203125" style="9" collapsed="1"/>
+    <col min="49" max="49" width="8.6640625" style="9" customWidth="1" collapsed="1"/>
+    <col min="50" max="56" width="8.83203125" style="9" collapsed="1"/>
+    <col min="57" max="57" width="8.83203125" style="9"/>
+    <col min="58" max="16384" width="8.83203125" style="9" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:56" ht="26.25" customHeight="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -661,7 +668,7 @@
         <v>41579</v>
       </c>
     </row>
-    <row r="2" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:56">
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
@@ -791,14 +798,11 @@
       <c r="AR2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AS2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AT2" s="11" t="s">
+      <c r="AS2" s="11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:56">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -931,33 +935,30 @@
       <c r="AR3" s="12">
         <v>29.055555555555557</v>
       </c>
-      <c r="AS3" s="12">
-        <v>5.4444444444444446</v>
-      </c>
-      <c r="AT3" s="13">
+      <c r="AS3" s="13">
         <v>4010.5555555555561</v>
       </c>
-      <c r="AU3" s="14"/>
-      <c r="AW3" s="9" t="s">
+      <c r="AT3" s="14"/>
+      <c r="AV3" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="AX3" s="24">
-        <f>SUM(B3:Z27,AK3:AN27,B38:Z41,AK38:AN41,B46:Z46,AS3:AS27,AS38:AS41,AK46:AN46,AS46)</f>
-        <v>85539.61111111092</v>
-      </c>
-      <c r="AZ3" s="9" t="s">
+      <c r="AW3" s="24" t="e">
+        <f>SUM(B3:Z27,AK3:AN27,B38:Z41,AK38:AN41,#REF!,#REF!,#REF!,#REF!,#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AY3" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="BA3" s="15">
-        <f>SUM(AX12:AX18,AY12:BD12)</f>
+      <c r="AZ3" s="15">
+        <f>SUM(AW12:AW18,AX12:BC12)</f>
         <v>250507.27777777781</v>
       </c>
-      <c r="BB3" s="16">
-        <f>BA3/BE$19</f>
+      <c r="BA3" s="16">
+        <f>AZ3/BD$19</f>
         <v>0.64485303812917116</v>
       </c>
     </row>
-    <row r="4" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:56">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1090,33 +1091,30 @@
       <c r="AR4" s="12">
         <v>56.166666666666664</v>
       </c>
-      <c r="AS4" s="12">
-        <v>17.666666666666668</v>
-      </c>
-      <c r="AT4" s="13">
+      <c r="AS4" s="13">
         <v>8648.4999999999982</v>
       </c>
-      <c r="AU4" s="14"/>
-      <c r="AW4" s="9" t="s">
+      <c r="AT4" s="14"/>
+      <c r="AV4" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="AX4" s="24">
+      <c r="AW4" s="24">
         <f>SUM(AA28:AJ37, AA42:AJ45, AO28:AR37, AO42:AR45)</f>
         <v>107744.05555555559</v>
       </c>
-      <c r="AZ4" s="9" t="s">
+      <c r="AY4" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="BA4" s="15">
-        <f>SUM(AY13:BC18)</f>
+      <c r="AZ4" s="15">
+        <f>SUM(AX13:BB18)</f>
         <v>129099.88888888885</v>
       </c>
-      <c r="BB4" s="16">
-        <f>BA4/BE$19</f>
+      <c r="BA4" s="16">
+        <f>AZ4/BD$19</f>
         <v>0.33232749288022262</v>
       </c>
     </row>
-    <row r="5" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:56">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1249,22 +1247,19 @@
       <c r="AR5" s="12">
         <v>25</v>
       </c>
-      <c r="AS5" s="12">
-        <v>10.777777777777779</v>
-      </c>
-      <c r="AT5" s="13">
+      <c r="AS5" s="13">
         <v>4755.5555555555566</v>
       </c>
-      <c r="AU5" s="14"/>
-      <c r="AW5" s="9" t="s">
+      <c r="AT5" s="14"/>
+      <c r="AV5" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="AX5" s="24">
-        <f>SUM(AA3:AJ27,B28:Z37,AA38:AJ41,AK28:AN37, B42:Z45, AK42:AN45, AO3:AR27, AO38:AR41,AS28:AS37,AS42:AS45,AA46:AJ46,AO46:AR46)</f>
-        <v>201613.61111111159</v>
+      <c r="AW5" s="24" t="e">
+        <f>SUM(AA3:AJ27,B28:Z37,AA38:AJ41,AK28:AN37, B42:Z45, AK42:AN45, AO3:AR27, AO38:AR41,#REF!,#REF!,#REF!,#REF!)</f>
+        <v>#REF!</v>
       </c>
     </row>
-    <row r="6" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:56">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1397,16 +1392,13 @@
       <c r="AR6" s="12">
         <v>35.055555555555557</v>
       </c>
-      <c r="AS6" s="12">
-        <v>6.666666666666667</v>
-      </c>
-      <c r="AT6" s="13">
+      <c r="AS6" s="13">
         <v>4676.7222222222217</v>
       </c>
-      <c r="AU6" s="14"/>
-      <c r="AX6" s="12"/>
+      <c r="AT6" s="14"/>
+      <c r="AW6" s="12"/>
     </row>
-    <row r="7" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:56">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1539,16 +1531,13 @@
       <c r="AR7" s="12">
         <v>165.16666666666666</v>
       </c>
-      <c r="AS7" s="12">
-        <v>54.722222222222221</v>
-      </c>
-      <c r="AT7" s="13">
+      <c r="AS7" s="13">
         <v>13223.444444444447</v>
       </c>
-      <c r="AU7" s="14"/>
-      <c r="AX7" s="12"/>
+      <c r="AT7" s="14"/>
+      <c r="AW7" s="12"/>
     </row>
-    <row r="8" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:56">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1681,16 +1670,13 @@
       <c r="AR8" s="12">
         <v>33.555555555555557</v>
       </c>
-      <c r="AS8" s="12">
-        <v>10.055555555555555</v>
-      </c>
-      <c r="AT8" s="13">
+      <c r="AS8" s="13">
         <v>5172.6111111111104</v>
       </c>
-      <c r="AU8" s="14"/>
-      <c r="AX8" s="15"/>
+      <c r="AT8" s="14"/>
+      <c r="AW8" s="15"/>
     </row>
-    <row r="9" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:56">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1823,16 +1809,13 @@
       <c r="AR9" s="12">
         <v>62.611111111111114</v>
       </c>
-      <c r="AS9" s="12">
-        <v>31</v>
-      </c>
-      <c r="AT9" s="13">
+      <c r="AS9" s="13">
         <v>8647.777777777781</v>
       </c>
-      <c r="AU9" s="14"/>
-      <c r="AX9" s="15"/>
+      <c r="AT9" s="14"/>
+      <c r="AW9" s="15"/>
     </row>
-    <row r="10" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:56">
       <c r="A10" s="1">
         <v>19</v>
       </c>
@@ -1965,18 +1948,15 @@
       <c r="AR10" s="12">
         <v>116.05555555555556</v>
       </c>
-      <c r="AS10" s="12">
-        <v>80.333333333333329</v>
-      </c>
-      <c r="AT10" s="13">
+      <c r="AS10" s="13">
         <v>11450.555555555557</v>
       </c>
-      <c r="AU10" s="14"/>
-      <c r="AW10" s="17"/>
-      <c r="AX10" s="15"/>
-      <c r="BD10" s="11"/>
+      <c r="AT10" s="14"/>
+      <c r="AV10" s="17"/>
+      <c r="AW10" s="15"/>
+      <c r="BC10" s="11"/>
     </row>
-    <row r="11" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:56">
       <c r="A11" s="1">
         <v>12</v>
       </c>
@@ -2109,40 +2089,37 @@
       <c r="AR11" s="12">
         <v>136.61111111111111</v>
       </c>
-      <c r="AS11" s="12">
-        <v>117.44444444444444</v>
-      </c>
-      <c r="AT11" s="13">
+      <c r="AS11" s="13">
         <v>12834.16666666667</v>
       </c>
-      <c r="AU11" s="14"/>
-      <c r="AW11" s="18"/>
+      <c r="AT11" s="14"/>
+      <c r="AV11" s="18"/>
+      <c r="AW11" s="15" t="s">
+        <v>43</v>
+      </c>
       <c r="AX11" s="15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AY11" s="15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AZ11" s="15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="BA11" s="15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="BB11" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="BC11" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="BD11" s="14" t="s">
+      <c r="BC11" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="BE11" s="15" t="s">
+      <c r="BD11" s="15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:56">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -2275,50 +2252,47 @@
       <c r="AR12" s="12">
         <v>21.666666666666668</v>
       </c>
-      <c r="AS12" s="12">
-        <v>79.722222222222229</v>
-      </c>
-      <c r="AT12" s="13">
+      <c r="AS12" s="13">
         <v>6740.9444444444462</v>
       </c>
-      <c r="AU12" s="14"/>
-      <c r="AW12" s="17" t="s">
+      <c r="AT12" s="14"/>
+      <c r="AV12" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="AX12" s="22">
+      <c r="AW12" s="22">
         <f>SUM(AA28:AD31)</f>
         <v>5554.3888888888887</v>
       </c>
-      <c r="AY12" s="22">
+      <c r="AX12" s="22">
         <f>SUM(Z28:Z31,H28:K31)</f>
         <v>18617.277777777777</v>
       </c>
-      <c r="AZ12" s="22">
+      <c r="AY12" s="22">
         <f>SUM(AE28:AJ31)</f>
         <v>32819.111111111117</v>
       </c>
-      <c r="BA12" s="22">
+      <c r="AZ12" s="22">
         <f>SUM(B28:G31)</f>
         <v>14363.444444444447</v>
       </c>
-      <c r="BB12" s="22">
+      <c r="BA12" s="22">
         <f>SUM(AM28:AN31,T28:Y31)</f>
         <v>21317.777777777777</v>
       </c>
-      <c r="BC12" s="22">
+      <c r="BB12" s="22">
         <f>SUM(AK28:AL31,L28:S31)</f>
         <v>24635.388888888891</v>
       </c>
-      <c r="BD12" s="23">
+      <c r="BC12" s="23">
         <f>SUM(AO28:AR31)</f>
         <v>10545</v>
       </c>
-      <c r="BE12" s="22">
-        <f t="shared" ref="BE12:BE19" si="0">SUM(AX12:BD12)</f>
+      <c r="BD12" s="22">
+        <f t="shared" ref="BD12:BD19" si="0">SUM(AW12:BC12)</f>
         <v>127852.38888888891</v>
       </c>
     </row>
-    <row r="13" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:56">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -2451,50 +2425,47 @@
       <c r="AR13" s="12">
         <v>30.333333333333332</v>
       </c>
-      <c r="AS13" s="12">
-        <v>50.722222222222221</v>
-      </c>
-      <c r="AT13" s="13">
+      <c r="AS13" s="13">
         <v>8173.8333333333321</v>
       </c>
-      <c r="AU13" s="14"/>
-      <c r="AW13" s="17" t="s">
+      <c r="AT13" s="14"/>
+      <c r="AV13" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="AX13" s="22">
+      <c r="AW13" s="22">
         <f>SUM(AA27:AD27,AA9:AD12)</f>
         <v>18694.444444444449</v>
       </c>
-      <c r="AY13" s="22">
+      <c r="AX13" s="22">
         <f>SUM(Z27,Z9:Z12,H9:K12,H27:K27)</f>
         <v>2035.4999999999998</v>
       </c>
-      <c r="AZ13" s="22">
+      <c r="AY13" s="22">
         <f>SUM(AE9:AJ12,AE27:AJ27)</f>
         <v>4590.8333333333321</v>
       </c>
-      <c r="BA13" s="22">
+      <c r="AZ13" s="22">
         <f>SUM(B9:G12,B27:G27)</f>
         <v>6212.6666666666661</v>
       </c>
-      <c r="BB13" s="22">
+      <c r="BA13" s="22">
         <f>SUM(T9:Y12,AM9:AN12,T27:Y27,AM27:AN27)</f>
         <v>4779.1111111111095</v>
       </c>
-      <c r="BC13" s="22">
+      <c r="BB13" s="22">
         <f>SUM(L9:S12,AK9:AL12,L27:S27,AK27:AL27)</f>
         <v>8278.4444444444489</v>
       </c>
-      <c r="BD13" s="23">
+      <c r="BC13" s="23">
         <f>SUM(AO9:AR12,AO27:AR27)</f>
         <v>1090.9444444444443</v>
       </c>
-      <c r="BE13" s="22">
+      <c r="BD13" s="22">
         <f t="shared" si="0"/>
         <v>45681.944444444445</v>
       </c>
     </row>
-    <row r="14" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:56">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -2627,50 +2598,47 @@
       <c r="AR14" s="12">
         <v>35.888888888888886</v>
       </c>
-      <c r="AS14" s="12">
-        <v>85.222222222222229</v>
-      </c>
-      <c r="AT14" s="13">
+      <c r="AS14" s="13">
         <v>7341.6666666666652</v>
       </c>
-      <c r="AU14" s="14"/>
-      <c r="AW14" s="17" t="s">
+      <c r="AT14" s="14"/>
+      <c r="AV14" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="AX14" s="22">
+      <c r="AW14" s="22">
         <f>SUM(AA32:AD37)</f>
         <v>31646.277777777785</v>
       </c>
-      <c r="AY14" s="22">
+      <c r="AX14" s="22">
         <f>SUM(H32:K37,Z32:Z37)</f>
         <v>4436.9444444444453</v>
       </c>
-      <c r="AZ14" s="22">
+      <c r="AY14" s="22">
         <f>SUM(AE32:AJ37)</f>
         <v>8570</v>
       </c>
-      <c r="BA14" s="22">
+      <c r="AZ14" s="22">
         <f>SUM(B32:G37)</f>
         <v>3421.0555555555552</v>
       </c>
-      <c r="BB14" s="22">
+      <c r="BA14" s="22">
         <f>SUM(T32:Y37,AM32:AN37)</f>
         <v>2459.1111111111122</v>
       </c>
-      <c r="BC14" s="22">
+      <c r="BB14" s="22">
         <f>SUM(L32:S37,AK32:AL37)</f>
         <v>3738.4444444444453</v>
       </c>
-      <c r="BD14" s="23">
+      <c r="BC14" s="23">
         <f>SUM(AO32:AR37)</f>
         <v>3218.1111111111113</v>
       </c>
-      <c r="BE14" s="22">
+      <c r="BD14" s="22">
         <f t="shared" si="0"/>
         <v>57489.944444444453</v>
       </c>
     </row>
-    <row r="15" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:56">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -2803,50 +2771,47 @@
       <c r="AR15" s="12">
         <v>20.222222222222221</v>
       </c>
-      <c r="AS15" s="12">
-        <v>44.944444444444443</v>
-      </c>
-      <c r="AT15" s="13">
+      <c r="AS15" s="13">
         <v>5748.4444444444443</v>
       </c>
-      <c r="AU15" s="14"/>
-      <c r="AW15" s="17" t="s">
+      <c r="AT15" s="14"/>
+      <c r="AV15" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="AX15" s="22">
+      <c r="AW15" s="22">
         <f>SUM(AA3:AD8)</f>
         <v>15380.111111111111</v>
       </c>
-      <c r="AY15" s="22">
+      <c r="AX15" s="22">
         <f>SUM(H3:K8,Z3:Z8)</f>
         <v>6369.6111111111104</v>
       </c>
-      <c r="AZ15" s="22">
+      <c r="AY15" s="22">
         <f>SUM(AE3:AJ8)</f>
         <v>3732.2777777777774</v>
       </c>
-      <c r="BA15" s="22">
+      <c r="AZ15" s="22">
         <f>SUM(B3:G8)</f>
         <v>7916.6111111111104</v>
       </c>
-      <c r="BB15" s="22">
+      <c r="BA15" s="22">
         <f>SUM(T3:Y8,AM3:AN8)</f>
         <v>1696.7777777777774</v>
       </c>
-      <c r="BC15" s="22">
+      <c r="BB15" s="22">
         <f>SUM(L3:S8,AK3:AL8)</f>
         <v>4216.3888888888887</v>
       </c>
-      <c r="BD15" s="23">
+      <c r="BC15" s="23">
         <f>SUM(AO3:AR8)</f>
         <v>1070.2777777777781</v>
       </c>
-      <c r="BE15" s="22">
+      <c r="BD15" s="22">
         <f t="shared" si="0"/>
         <v>40382.055555555562</v>
       </c>
     </row>
-    <row r="16" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:56">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -2979,50 +2944,47 @@
       <c r="AR16" s="12">
         <v>11.277777777777779</v>
       </c>
-      <c r="AS16" s="12">
-        <v>119.5</v>
-      </c>
-      <c r="AT16" s="13">
+      <c r="AS16" s="13">
         <v>5787.7222222222208</v>
       </c>
-      <c r="AU16" s="14"/>
-      <c r="AW16" s="17" t="s">
+      <c r="AT16" s="14"/>
+      <c r="AV16" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="AX16" s="22">
+      <c r="AW16" s="22">
         <f>SUM(AA21:AD26,AA40:AD41)</f>
         <v>21827.333333333325</v>
       </c>
-      <c r="AY16" s="22">
+      <c r="AX16" s="22">
         <f>SUM(H21:K26,H40:K41,Z21:Z26,Z40:Z41)</f>
         <v>4859.666666666667</v>
       </c>
-      <c r="AZ16" s="22">
+      <c r="AY16" s="22">
         <f>SUM(AE21:AJ26,AE40:AJ41)</f>
         <v>2715.1666666666661</v>
       </c>
-      <c r="BA16" s="22">
+      <c r="AZ16" s="22">
         <f>SUM(B21:G26,B40:G41)</f>
         <v>1714.4444444444441</v>
       </c>
-      <c r="BB16" s="22">
+      <c r="BA16" s="22">
         <f>SUM(T21:Y26,T40:Y41,AM21:AN26,AM40:AN41)</f>
         <v>5679.7222222222199</v>
       </c>
-      <c r="BC16" s="22">
+      <c r="BB16" s="22">
         <f>SUM(L21:S26,L40:S41,AK21:AL26,AK40:AL41)</f>
         <v>1833.1111111111106</v>
       </c>
-      <c r="BD16" s="23">
+      <c r="BC16" s="23">
         <f>SUM(AO21:AR26,AO40:AR41)</f>
         <v>1287.4444444444443</v>
       </c>
-      <c r="BE16" s="22">
+      <c r="BD16" s="22">
         <f t="shared" si="0"/>
         <v>39916.888888888876</v>
       </c>
     </row>
-    <row r="17" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:56">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -3155,50 +3117,47 @@
       <c r="AR17" s="12">
         <v>9.0555555555555554</v>
       </c>
-      <c r="AS17" s="12">
-        <v>51.555555555555557</v>
-      </c>
-      <c r="AT17" s="13">
+      <c r="AS17" s="13">
         <v>5288.6111111111113</v>
       </c>
-      <c r="AU17" s="14"/>
-      <c r="AW17" s="1" t="s">
+      <c r="AT17" s="14"/>
+      <c r="AV17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AX17" s="23">
+      <c r="AW17" s="23">
         <f>SUM(AA13:AD20,AA38:AD39)</f>
         <v>24583.888888888887</v>
       </c>
-      <c r="AY17" s="23">
+      <c r="AX17" s="23">
         <f>SUM(H13:K20,H38:K39,Z13:Z20,Z38:Z39)</f>
         <v>8360.0555555555547</v>
       </c>
-      <c r="AZ17" s="23">
+      <c r="AY17" s="23">
         <f>SUM(AE13:AJ20,AE38:AJ39)</f>
         <v>3919.4444444444448</v>
       </c>
-      <c r="BA17" s="23">
+      <c r="AZ17" s="23">
         <f>SUM(B13:G20,B38:G39)</f>
         <v>4477.2222222222235</v>
       </c>
-      <c r="BB17" s="23">
+      <c r="BA17" s="23">
         <f>SUM(T13:Y20,T38:Y39,AM13:AN20,AM38:AN39)</f>
         <v>1868.3888888888882</v>
       </c>
-      <c r="BC17" s="23">
+      <c r="BB17" s="23">
         <f>SUM(L13:S20,L38:S39,AK13:AL20,AK38:AL39)</f>
         <v>13126.5</v>
       </c>
-      <c r="BD17" s="23">
+      <c r="BC17" s="23">
         <f>SUM(AO13:AR20,AO38:AR39)</f>
         <v>824.55555555555532</v>
       </c>
-      <c r="BE17" s="22">
+      <c r="BD17" s="22">
         <f t="shared" si="0"/>
         <v>57160.055555555555</v>
       </c>
     </row>
-    <row r="18" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:56">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -3331,50 +3290,47 @@
       <c r="AR18" s="12">
         <v>5</v>
       </c>
-      <c r="AS18" s="12">
-        <v>24.777777777777779</v>
-      </c>
-      <c r="AT18" s="13">
+      <c r="AS18" s="13">
         <v>3097.9444444444448</v>
       </c>
-      <c r="AU18" s="14"/>
-      <c r="AW18" s="9" t="s">
+      <c r="AT18" s="14"/>
+      <c r="AV18" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="AX18" s="22">
+      <c r="AW18" s="22">
         <f>SUM(AA42:AD45)</f>
         <v>10522.833333333332</v>
       </c>
-      <c r="AY18" s="22">
+      <c r="AX18" s="22">
         <f>SUM(Z42:Z45,H42:K45)</f>
         <v>1194.7222222222222</v>
       </c>
-      <c r="AZ18" s="22">
+      <c r="AY18" s="22">
         <f>SUM(AE42:AJ45)</f>
         <v>3494.9444444444448</v>
       </c>
-      <c r="BA18" s="22">
+      <c r="AZ18" s="22">
         <f>SUM(B42:G45)</f>
         <v>1273.9444444444443</v>
       </c>
-      <c r="BB18" s="22">
+      <c r="BA18" s="22">
         <f>SUM(T42:Y45, AM42:AN45)</f>
         <v>1328.9444444444443</v>
       </c>
-      <c r="BC18" s="22">
+      <c r="BB18" s="22">
         <f>SUM(AK42:AL45,L42:S45)</f>
         <v>799.83333333333337</v>
       </c>
-      <c r="BD18" s="22">
+      <c r="BC18" s="22">
         <f>SUM(AO42:AR45)</f>
         <v>1373.3888888888887</v>
       </c>
-      <c r="BE18" s="22">
+      <c r="BD18" s="22">
         <f t="shared" si="0"/>
         <v>19988.611111111109</v>
       </c>
     </row>
-    <row r="19" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:56">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -3507,50 +3463,47 @@
       <c r="AR19" s="12">
         <v>4.8888888888888893</v>
       </c>
-      <c r="AS19" s="12">
-        <v>30.111111111111111</v>
-      </c>
-      <c r="AT19" s="13">
+      <c r="AS19" s="13">
         <v>4556.8333333333321</v>
       </c>
-      <c r="AU19" s="14"/>
-      <c r="AW19" s="9" t="s">
+      <c r="AT19" s="14"/>
+      <c r="AV19" s="9" t="s">
         <v>49</v>
       </c>
+      <c r="AW19" s="22">
+        <f>SUM(AW12:AW18)</f>
+        <v>128209.27777777778</v>
+      </c>
       <c r="AX19" s="22">
-        <f>SUM(AX12:AX18)</f>
-        <v>128209.27777777778</v>
+        <f t="shared" ref="AX19:BC19" si="1">SUM(AX12:AX18)</f>
+        <v>45873.777777777774</v>
       </c>
       <c r="AY19" s="22">
-        <f t="shared" ref="AY19:BD19" si="1">SUM(AY12:AY18)</f>
-        <v>45873.777777777774</v>
+        <f t="shared" si="1"/>
+        <v>59841.777777777788</v>
       </c>
       <c r="AZ19" s="22">
         <f t="shared" si="1"/>
-        <v>59841.777777777788</v>
+        <v>39379.388888888891</v>
       </c>
       <c r="BA19" s="22">
         <f t="shared" si="1"/>
-        <v>39379.388888888891</v>
+        <v>39129.833333333336</v>
       </c>
       <c r="BB19" s="22">
         <f t="shared" si="1"/>
-        <v>39129.833333333336</v>
+        <v>56628.111111111124</v>
       </c>
       <c r="BC19" s="22">
         <f t="shared" si="1"/>
-        <v>56628.111111111124</v>
+        <v>19409.722222222219</v>
       </c>
       <c r="BD19" s="22">
-        <f t="shared" si="1"/>
-        <v>19409.722222222219</v>
-      </c>
-      <c r="BE19" s="22">
         <f t="shared" si="0"/>
         <v>388471.88888888888</v>
       </c>
     </row>
-    <row r="20" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:56">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -3683,14 +3636,12 @@
       <c r="AR20" s="12">
         <v>9.2777777777777786</v>
       </c>
-      <c r="AS20" s="12">
-        <v>36.333333333333336</v>
-      </c>
-      <c r="AT20" s="13">
+      <c r="AS20" s="13">
         <v>8256.5</v>
       </c>
-      <c r="AU20" s="14"/>
-      <c r="AW20" s="18"/>
+      <c r="AT20" s="14"/>
+      <c r="AV20" s="18"/>
+      <c r="AW20" s="22"/>
       <c r="AX20" s="22"/>
       <c r="AY20" s="22"/>
       <c r="AZ20" s="22"/>
@@ -3698,9 +3649,8 @@
       <c r="BB20" s="22"/>
       <c r="BC20" s="22"/>
       <c r="BD20" s="22"/>
-      <c r="BE20" s="22"/>
     </row>
-    <row r="21" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:56">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
@@ -3833,38 +3783,35 @@
       <c r="AR21" s="12">
         <v>24.388888888888889</v>
       </c>
-      <c r="AS21" s="12">
-        <v>7.166666666666667</v>
-      </c>
-      <c r="AT21" s="13">
+      <c r="AS21" s="13">
         <v>5948.5555555555566</v>
       </c>
-      <c r="AU21" s="14"/>
-      <c r="AW21" s="17"/>
+      <c r="AT21" s="14"/>
+      <c r="AV21" s="17"/>
+      <c r="AW21" s="22" t="s">
+        <v>43</v>
+      </c>
       <c r="AX21" s="22" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AY21" s="22" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AZ21" s="22" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="BA21" s="22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="BB21" s="22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="BC21" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="BD21" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="BE21" s="22"/>
+      <c r="BD21" s="22"/>
     </row>
-    <row r="22" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:56">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -3997,29 +3944,26 @@
       <c r="AR22" s="12">
         <v>23.055555555555557</v>
       </c>
-      <c r="AS22" s="12">
-        <v>3.2777777777777777</v>
-      </c>
-      <c r="AT22" s="13">
+      <c r="AS22" s="13">
         <v>6504.9444444444462</v>
       </c>
-      <c r="AU22" s="14"/>
-      <c r="AW22" s="17" t="s">
+      <c r="AT22" s="14"/>
+      <c r="AV22" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="AX22" s="22">
-        <f>AX12</f>
+      <c r="AW22" s="22">
+        <f>AW12</f>
         <v>5554.3888888888887</v>
       </c>
+      <c r="AX22" s="22"/>
       <c r="AY22" s="22"/>
       <c r="AZ22" s="22"/>
       <c r="BA22" s="22"/>
       <c r="BB22" s="22"/>
       <c r="BC22" s="22"/>
       <c r="BD22" s="22"/>
-      <c r="BE22" s="22"/>
     </row>
-    <row r="23" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:56">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
@@ -4152,32 +4096,29 @@
       <c r="AR23" s="12">
         <v>28.444444444444443</v>
       </c>
-      <c r="AS23" s="12">
-        <v>4.4444444444444446</v>
-      </c>
-      <c r="AT23" s="13">
+      <c r="AS23" s="13">
         <v>6527.9444444444416</v>
       </c>
-      <c r="AU23" s="14"/>
-      <c r="AW23" s="17" t="s">
+      <c r="AT23" s="14"/>
+      <c r="AV23" s="17" t="s">
         <v>44</v>
       </c>
+      <c r="AW23" s="22">
+        <f>AW13+AX12</f>
+        <v>37311.722222222226</v>
+      </c>
       <c r="AX23" s="22">
-        <f>AX13+AY12</f>
-        <v>37311.722222222226</v>
-      </c>
-      <c r="AY23" s="22">
-        <f>AY13</f>
+        <f>AX13</f>
         <v>2035.4999999999998</v>
       </c>
+      <c r="AY23" s="22"/>
       <c r="AZ23" s="22"/>
       <c r="BA23" s="22"/>
       <c r="BB23" s="22"/>
       <c r="BC23" s="22"/>
       <c r="BD23" s="22"/>
-      <c r="BE23" s="22"/>
     </row>
-    <row r="24" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:56">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -4310,35 +4251,32 @@
       <c r="AR24" s="12">
         <v>13.444444444444445</v>
       </c>
-      <c r="AS24" s="12">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="AT24" s="13">
+      <c r="AS24" s="13">
         <v>3669.9444444444439</v>
       </c>
-      <c r="AU24" s="14"/>
-      <c r="AW24" s="17" t="s">
+      <c r="AT24" s="14"/>
+      <c r="AV24" s="17" t="s">
         <v>45</v>
       </c>
+      <c r="AW24" s="22">
+        <f>AW14+AY12</f>
+        <v>64465.388888888905</v>
+      </c>
       <c r="AX24" s="22">
-        <f>AX14+AZ12</f>
-        <v>64465.388888888905</v>
+        <f>AX14+AY13</f>
+        <v>9027.7777777777774</v>
       </c>
       <c r="AY24" s="22">
-        <f>AY14+AZ13</f>
-        <v>9027.7777777777774</v>
-      </c>
-      <c r="AZ24" s="22">
-        <f>AZ14</f>
+        <f>AY14</f>
         <v>8570</v>
       </c>
+      <c r="AZ24" s="22"/>
       <c r="BA24" s="22"/>
       <c r="BB24" s="22"/>
       <c r="BC24" s="22"/>
       <c r="BD24" s="22"/>
-      <c r="BE24" s="22"/>
     </row>
-    <row r="25" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:56">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
@@ -4471,38 +4409,35 @@
       <c r="AR25" s="12">
         <v>10.5</v>
       </c>
-      <c r="AS25" s="12">
-        <v>1.2222222222222223</v>
-      </c>
-      <c r="AT25" s="13">
+      <c r="AS25" s="13">
         <v>2886.7777777777769</v>
       </c>
-      <c r="AU25" s="14"/>
-      <c r="AW25" s="17" t="s">
+      <c r="AT25" s="14"/>
+      <c r="AV25" s="17" t="s">
         <v>46</v>
       </c>
+      <c r="AW25" s="22">
+        <f>AW15+AZ12</f>
+        <v>29743.555555555558</v>
+      </c>
       <c r="AX25" s="22">
-        <f>AX15+BA12</f>
-        <v>29743.555555555558</v>
+        <f>AX15+AZ13</f>
+        <v>12582.277777777777</v>
       </c>
       <c r="AY25" s="22">
-        <f>AY15+BA13</f>
-        <v>12582.277777777777</v>
+        <f>AY15+AZ14</f>
+        <v>7153.3333333333321</v>
       </c>
       <c r="AZ25" s="22">
-        <f>AZ15+BA14</f>
-        <v>7153.3333333333321</v>
-      </c>
-      <c r="BA25" s="22">
-        <f>BA15</f>
+        <f>AZ15</f>
         <v>7916.6111111111104</v>
       </c>
+      <c r="BA25" s="22"/>
       <c r="BB25" s="22"/>
-      <c r="BC25" s="22"/>
-      <c r="BD25" s="23"/>
-      <c r="BE25" s="22"/>
+      <c r="BC25" s="23"/>
+      <c r="BD25" s="22"/>
     </row>
-    <row r="26" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:56">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -4635,41 +4570,38 @@
       <c r="AR26" s="12">
         <v>23.166666666666668</v>
       </c>
-      <c r="AS26" s="12">
-        <v>6.166666666666667</v>
-      </c>
-      <c r="AT26" s="13">
+      <c r="AS26" s="13">
         <v>6061.333333333333</v>
       </c>
-      <c r="AU26" s="14"/>
-      <c r="AW26" s="9" t="s">
+      <c r="AT26" s="14"/>
+      <c r="AV26" s="9" t="s">
         <v>47</v>
       </c>
+      <c r="AW26" s="22">
+        <f>AW16+BA12</f>
+        <v>43145.111111111102</v>
+      </c>
       <c r="AX26" s="22">
-        <f>AX16+BB12</f>
-        <v>43145.111111111102</v>
+        <f>AX16+BA13</f>
+        <v>9638.7777777777774</v>
       </c>
       <c r="AY26" s="22">
-        <f>AY16+BB13</f>
-        <v>9638.7777777777774</v>
+        <f>AY16+BA14</f>
+        <v>5174.2777777777783</v>
       </c>
       <c r="AZ26" s="22">
-        <f>AZ16+BB14</f>
-        <v>5174.2777777777783</v>
+        <f>AZ16+BA15</f>
+        <v>3411.2222222222217</v>
       </c>
       <c r="BA26" s="22">
-        <f>BA16+BB15</f>
-        <v>3411.2222222222217</v>
-      </c>
-      <c r="BB26" s="22">
-        <f>BB16</f>
+        <f>BA16</f>
         <v>5679.7222222222199</v>
       </c>
+      <c r="BB26" s="22"/>
       <c r="BC26" s="22"/>
       <c r="BD26" s="22"/>
-      <c r="BE26" s="22"/>
     </row>
-    <row r="27" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:56">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
@@ -4802,44 +4734,41 @@
       <c r="AR27" s="12">
         <v>23</v>
       </c>
-      <c r="AS27" s="12">
-        <v>8.1666666666666661</v>
-      </c>
-      <c r="AT27" s="13">
+      <c r="AS27" s="13">
         <v>6325.1666666666661</v>
       </c>
-      <c r="AU27" s="14"/>
-      <c r="AW27" s="9" t="s">
+      <c r="AT27" s="14"/>
+      <c r="AV27" s="9" t="s">
         <v>48</v>
       </c>
+      <c r="AW27" s="22">
+        <f>AW17+BB12</f>
+        <v>49219.277777777781</v>
+      </c>
       <c r="AX27" s="22">
-        <f>AX17+BC12</f>
-        <v>49219.277777777781</v>
+        <f>AX17+BB13</f>
+        <v>16638.500000000004</v>
       </c>
       <c r="AY27" s="22">
-        <f>AY17+BC13</f>
-        <v>16638.500000000004</v>
+        <f>AY17+BB14</f>
+        <v>7657.8888888888905</v>
       </c>
       <c r="AZ27" s="22">
-        <f>AZ17+BC14</f>
-        <v>7657.8888888888905</v>
+        <f>AZ17+BB15</f>
+        <v>8693.6111111111131</v>
       </c>
       <c r="BA27" s="22">
-        <f>BA17+BC15</f>
-        <v>8693.6111111111131</v>
+        <f>BA17+BB16</f>
+        <v>3701.4999999999991</v>
       </c>
       <c r="BB27" s="22">
-        <f>BB17+BC16</f>
-        <v>3701.4999999999991</v>
-      </c>
-      <c r="BC27" s="22">
-        <f>BC17</f>
+        <f>BB17</f>
         <v>13126.5</v>
       </c>
+      <c r="BC27" s="22"/>
       <c r="BD27" s="22"/>
-      <c r="BE27" s="22"/>
     </row>
-    <row r="28" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:56">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -4972,50 +4901,47 @@
       <c r="AR28" s="12">
         <v>978.66666666666663</v>
       </c>
-      <c r="AS28" s="12">
-        <v>807.05555555555554</v>
-      </c>
-      <c r="AT28" s="13">
+      <c r="AS28" s="13">
         <v>40248.55555555554</v>
       </c>
-      <c r="AU28" s="14"/>
-      <c r="AW28" s="9" t="s">
+      <c r="AT28" s="14"/>
+      <c r="AV28" s="9" t="s">
         <v>58</v>
       </c>
+      <c r="AW28" s="22">
+        <f>AW18+BC12</f>
+        <v>21067.833333333332</v>
+      </c>
       <c r="AX28" s="22">
-        <f>AX18+BD12</f>
-        <v>21067.833333333332</v>
+        <f>AX18+BC13</f>
+        <v>2285.6666666666665</v>
       </c>
       <c r="AY28" s="22">
-        <f>AY18+BD13</f>
-        <v>2285.6666666666665</v>
+        <f>AY18+BC14</f>
+        <v>6713.0555555555566</v>
       </c>
       <c r="AZ28" s="22">
-        <f>AZ18+BD14</f>
-        <v>6713.0555555555566</v>
+        <f>AZ18+BC15</f>
+        <v>2344.2222222222226</v>
       </c>
       <c r="BA28" s="22">
-        <f>BA18+BD15</f>
-        <v>2344.2222222222226</v>
+        <f>BA18+BC16</f>
+        <v>2616.3888888888887</v>
       </c>
       <c r="BB28" s="22">
-        <f>BB18+BD16</f>
-        <v>2616.3888888888887</v>
+        <f>SUM(BB18,BC17)</f>
+        <v>1624.3888888888887</v>
       </c>
       <c r="BC28" s="22">
-        <f>SUM(BC18,BD17)</f>
-        <v>1624.3888888888887</v>
+        <f>BC18</f>
+        <v>1373.3888888888887</v>
       </c>
       <c r="BD28" s="22">
-        <f>BD18</f>
-        <v>1373.3888888888887</v>
-      </c>
-      <c r="BE28" s="22">
-        <f>SUM(AX22:BD28)</f>
+        <f>SUM(AW22:BC28)</f>
         <v>388471.88888888893</v>
       </c>
     </row>
-    <row r="29" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:56">
       <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
@@ -5148,16 +5074,13 @@
       <c r="AR29" s="12">
         <v>1358.3333333333333</v>
       </c>
-      <c r="AS29" s="12">
-        <v>606.77777777777783</v>
-      </c>
-      <c r="AT29" s="13">
+      <c r="AS29" s="13">
         <v>40098.555555555562</v>
       </c>
-      <c r="AU29" s="14"/>
-      <c r="AX29" s="15"/>
+      <c r="AT29" s="14"/>
+      <c r="AW29" s="15"/>
     </row>
-    <row r="30" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:56">
       <c r="A30" s="1" t="s">
         <v>27</v>
       </c>
@@ -5290,16 +5213,13 @@
       <c r="AR30" s="12">
         <v>760.72222222222217</v>
       </c>
-      <c r="AS30" s="12">
-        <v>302.11111111111109</v>
-      </c>
-      <c r="AT30" s="13">
+      <c r="AS30" s="13">
         <v>28818.999999999993</v>
       </c>
-      <c r="AU30" s="14"/>
-      <c r="AX30" s="15"/>
+      <c r="AT30" s="14"/>
+      <c r="AW30" s="15"/>
     </row>
-    <row r="31" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:56">
       <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
@@ -5432,16 +5352,13 @@
       <c r="AR31" s="12">
         <v>499.27777777777777</v>
       </c>
-      <c r="AS31" s="12">
-        <v>204.44444444444446</v>
-      </c>
-      <c r="AT31" s="13">
+      <c r="AS31" s="13">
         <v>20606.666666666672</v>
       </c>
-      <c r="AU31" s="14"/>
-      <c r="AX31" s="15"/>
+      <c r="AT31" s="14"/>
+      <c r="AW31" s="15"/>
     </row>
-    <row r="32" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:56">
       <c r="A32" s="1">
         <v>16</v>
       </c>
@@ -5574,16 +5491,13 @@
       <c r="AR32" s="12">
         <v>231.5</v>
       </c>
-      <c r="AS32" s="12">
-        <v>39.888888888888886</v>
-      </c>
-      <c r="AT32" s="13">
+      <c r="AS32" s="13">
         <v>11884.111111111106</v>
       </c>
-      <c r="AU32" s="14"/>
-      <c r="AX32" s="15"/>
+      <c r="AT32" s="14"/>
+      <c r="AW32" s="15"/>
     </row>
-    <row r="33" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:49">
       <c r="A33" s="1">
         <v>24</v>
       </c>
@@ -5716,16 +5630,13 @@
       <c r="AR33" s="12">
         <v>245.61111111111111</v>
       </c>
-      <c r="AS33" s="12">
-        <v>32.333333333333336</v>
-      </c>
-      <c r="AT33" s="13">
+      <c r="AS33" s="13">
         <v>12560.722222222223</v>
       </c>
-      <c r="AU33" s="14"/>
-      <c r="AX33" s="15"/>
+      <c r="AT33" s="14"/>
+      <c r="AW33" s="15"/>
     </row>
-    <row r="34" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:49">
       <c r="A34" s="1" t="s">
         <v>29</v>
       </c>
@@ -5858,16 +5769,13 @@
       <c r="AR34" s="12">
         <v>148.61111111111111</v>
       </c>
-      <c r="AS34" s="12">
-        <v>16.888888888888889</v>
-      </c>
-      <c r="AT34" s="13">
+      <c r="AS34" s="13">
         <v>7371.8333333333339</v>
       </c>
-      <c r="AU34" s="14"/>
-      <c r="AX34" s="15"/>
+      <c r="AT34" s="14"/>
+      <c r="AW34" s="15"/>
     </row>
-    <row r="35" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:49">
       <c r="A35" s="1" t="s">
         <v>30</v>
       </c>
@@ -6000,16 +5908,13 @@
       <c r="AR35" s="12">
         <v>173.11111111111111</v>
       </c>
-      <c r="AS35" s="12">
-        <v>20.333333333333332</v>
-      </c>
-      <c r="AT35" s="13">
+      <c r="AS35" s="13">
         <v>11975.555555555555</v>
       </c>
-      <c r="AU35" s="14"/>
-      <c r="AX35" s="15"/>
+      <c r="AT35" s="14"/>
+      <c r="AW35" s="15"/>
     </row>
-    <row r="36" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:49">
       <c r="A36" s="1" t="s">
         <v>31</v>
       </c>
@@ -6142,16 +6047,13 @@
       <c r="AR36" s="12">
         <v>288.33333333333331</v>
       </c>
-      <c r="AS36" s="12">
-        <v>51.5</v>
-      </c>
-      <c r="AT36" s="13">
+      <c r="AS36" s="13">
         <v>9493.777777777781</v>
       </c>
-      <c r="AU36" s="14"/>
-      <c r="AX36" s="15"/>
+      <c r="AT36" s="14"/>
+      <c r="AW36" s="15"/>
     </row>
-    <row r="37" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:49">
       <c r="A37" s="1" t="s">
         <v>32</v>
       </c>
@@ -6284,16 +6186,13 @@
       <c r="AR37" s="12">
         <v>119.05555555555556</v>
       </c>
-      <c r="AS37" s="12">
-        <v>3.6111111111111112</v>
-      </c>
-      <c r="AT37" s="13">
+      <c r="AS37" s="13">
         <v>4368.5</v>
       </c>
-      <c r="AU37" s="14"/>
-      <c r="AX37" s="15"/>
+      <c r="AT37" s="14"/>
+      <c r="AW37" s="15"/>
     </row>
-    <row r="38" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:49">
       <c r="A38" s="1" t="s">
         <v>33</v>
       </c>
@@ -6426,16 +6325,13 @@
       <c r="AR38" s="12">
         <v>5.1111111111111107</v>
       </c>
-      <c r="AS38" s="12">
-        <v>92</v>
-      </c>
-      <c r="AT38" s="13">
+      <c r="AS38" s="13">
         <v>2695.1666666666665</v>
       </c>
-      <c r="AU38" s="14"/>
-      <c r="AX38" s="15"/>
+      <c r="AT38" s="14"/>
+      <c r="AW38" s="15"/>
     </row>
-    <row r="39" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:49">
       <c r="A39" s="1" t="s">
         <v>34</v>
       </c>
@@ -6568,16 +6464,13 @@
       <c r="AR39" s="12">
         <v>21.055555555555557</v>
       </c>
-      <c r="AS39" s="12">
-        <v>30.611111111111111</v>
-      </c>
-      <c r="AT39" s="13">
+      <c r="AS39" s="13">
         <v>6779.1111111111113</v>
       </c>
-      <c r="AU39" s="14"/>
-      <c r="AX39" s="15"/>
+      <c r="AT39" s="14"/>
+      <c r="AW39" s="15"/>
     </row>
-    <row r="40" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:49">
       <c r="A40" s="1" t="s">
         <v>35</v>
       </c>
@@ -6710,16 +6603,13 @@
       <c r="AR40" s="12">
         <v>11.611111111111111</v>
       </c>
-      <c r="AS40" s="12">
-        <v>2.0555555555555554</v>
-      </c>
-      <c r="AT40" s="13">
+      <c r="AS40" s="13">
         <v>2629.2777777777783</v>
       </c>
-      <c r="AU40" s="14"/>
-      <c r="AX40" s="15"/>
+      <c r="AT40" s="14"/>
+      <c r="AW40" s="15"/>
     </row>
-    <row r="41" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:49">
       <c r="A41" s="1" t="s">
         <v>36</v>
       </c>
@@ -6852,16 +6742,13 @@
       <c r="AR41" s="12">
         <v>37.222222222222221</v>
       </c>
-      <c r="AS41" s="12">
-        <v>8.6111111111111107</v>
-      </c>
-      <c r="AT41" s="13">
+      <c r="AS41" s="13">
         <v>5721.7222222222235</v>
       </c>
-      <c r="AU41" s="14"/>
-      <c r="AX41" s="15"/>
+      <c r="AT41" s="14"/>
+      <c r="AW41" s="15"/>
     </row>
-    <row r="42" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:49">
       <c r="A42" s="1" t="s">
         <v>53</v>
       </c>
@@ -6994,16 +6881,13 @@
       <c r="AR42" s="12">
         <v>64.777777777777771</v>
       </c>
-      <c r="AS42" s="12">
-        <v>4.4444444444444446</v>
-      </c>
-      <c r="AT42" s="13">
+      <c r="AS42" s="13">
         <v>3268.2777777777778</v>
       </c>
-      <c r="AU42" s="14"/>
-      <c r="AX42" s="15"/>
+      <c r="AT42" s="14"/>
+      <c r="AW42" s="15"/>
     </row>
-    <row r="43" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:49">
       <c r="A43" s="1" t="s">
         <v>54</v>
       </c>
@@ -7136,16 +7020,13 @@
       <c r="AR43" s="12">
         <v>81</v>
       </c>
-      <c r="AS43" s="12">
-        <v>3.5555555555555554</v>
-      </c>
-      <c r="AT43" s="13">
+      <c r="AS43" s="13">
         <v>3607.8888888888896</v>
       </c>
-      <c r="AU43" s="14"/>
-      <c r="AX43" s="15"/>
+      <c r="AT43" s="14"/>
+      <c r="AW43" s="15"/>
     </row>
-    <row r="44" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:49">
       <c r="A44" s="1" t="s">
         <v>55</v>
       </c>
@@ -7278,16 +7159,13 @@
       <c r="AR44" s="12">
         <v>397.61111111111109</v>
       </c>
-      <c r="AS44" s="12">
-        <v>36.388888888888886</v>
-      </c>
-      <c r="AT44" s="13">
+      <c r="AS44" s="13">
         <v>6985.5555555555557</v>
       </c>
-      <c r="AU44" s="14"/>
-      <c r="AX44" s="15"/>
+      <c r="AT44" s="14"/>
+      <c r="AW44" s="15"/>
     </row>
-    <row r="45" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:49">
       <c r="A45" s="1" t="s">
         <v>56</v>
       </c>
@@ -7420,362 +7298,219 @@
       <c r="AR45" s="12">
         <v>33.333333333333336</v>
       </c>
-      <c r="AS45" s="12">
-        <v>7.2222222222222223</v>
-      </c>
-      <c r="AT45" s="13">
+      <c r="AS45" s="13">
         <v>6178.5000000000009</v>
       </c>
-      <c r="AU45" s="14"/>
-      <c r="AX45" s="15"/>
+      <c r="AT45" s="14"/>
+      <c r="AW45" s="15"/>
     </row>
-    <row r="46" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B46" s="12">
-        <v>6</v>
-      </c>
-      <c r="C46" s="12">
-        <v>19.555555555555557</v>
-      </c>
-      <c r="D46" s="12">
-        <v>9.7222222222222214</v>
-      </c>
-      <c r="E46" s="12">
-        <v>8.3333333333333339</v>
-      </c>
-      <c r="F46" s="12">
-        <v>59.5</v>
-      </c>
-      <c r="G46" s="12">
-        <v>11.166666666666666</v>
-      </c>
-      <c r="H46" s="12">
-        <v>33.388888888888886</v>
-      </c>
-      <c r="I46" s="12">
-        <v>81.611111111111114</v>
-      </c>
-      <c r="J46" s="12">
-        <v>118.38888888888889</v>
-      </c>
-      <c r="K46" s="12">
-        <v>82.611111111111114</v>
-      </c>
-      <c r="L46" s="12">
-        <v>56.111111111111114</v>
-      </c>
-      <c r="M46" s="12">
-        <v>92.444444444444443</v>
-      </c>
-      <c r="N46" s="12">
-        <v>51.333333333333336</v>
-      </c>
-      <c r="O46" s="12">
-        <v>127.11111111111111</v>
-      </c>
-      <c r="P46" s="12">
-        <v>47.944444444444443</v>
-      </c>
-      <c r="Q46" s="12">
-        <v>31.444444444444443</v>
-      </c>
-      <c r="R46" s="12">
-        <v>30.277777777777779</v>
-      </c>
-      <c r="S46" s="12">
-        <v>39.388888888888886</v>
-      </c>
-      <c r="T46" s="12">
-        <v>5.4444444444444446</v>
-      </c>
-      <c r="U46" s="12">
-        <v>5.7777777777777777</v>
-      </c>
-      <c r="V46" s="12">
-        <v>4.166666666666667</v>
-      </c>
-      <c r="W46" s="12">
-        <v>1.0555555555555556</v>
-      </c>
-      <c r="X46" s="12">
-        <v>1.2777777777777777</v>
-      </c>
-      <c r="Y46" s="12">
-        <v>7.666666666666667</v>
-      </c>
-      <c r="Z46" s="12">
-        <v>11.333333333333334</v>
-      </c>
-      <c r="AA46" s="12">
-        <v>727.33333333333337</v>
-      </c>
-      <c r="AB46" s="12">
-        <v>620.38888888888891</v>
-      </c>
-      <c r="AC46" s="12">
-        <v>353.27777777777777</v>
-      </c>
-      <c r="AD46" s="12">
-        <v>237.11111111111111</v>
-      </c>
-      <c r="AE46" s="12">
-        <v>47.388888888888886</v>
-      </c>
-      <c r="AF46" s="12">
-        <v>35</v>
-      </c>
-      <c r="AG46" s="12">
-        <v>18.388888888888889</v>
-      </c>
-      <c r="AH46" s="12">
-        <v>18.611111111111111</v>
-      </c>
-      <c r="AI46" s="12">
-        <v>54.833333333333336</v>
-      </c>
-      <c r="AJ46" s="12">
-        <v>4.6111111111111107</v>
-      </c>
-      <c r="AK46" s="12">
-        <v>99.5</v>
-      </c>
-      <c r="AL46" s="12">
-        <v>26.333333333333332</v>
-      </c>
-      <c r="AM46" s="12">
-        <v>2</v>
-      </c>
-      <c r="AN46" s="12">
-        <v>9.7777777777777786</v>
-      </c>
-      <c r="AO46" s="12">
-        <v>5.333333333333333</v>
-      </c>
-      <c r="AP46" s="12">
-        <v>3.2777777777777777</v>
-      </c>
-      <c r="AQ46" s="12">
-        <v>40.833333333333336</v>
-      </c>
-      <c r="AR46" s="12">
-        <v>7.0555555555555554</v>
-      </c>
-      <c r="AS46" s="12">
-        <v>13.333333333333334</v>
-      </c>
-      <c r="AT46" s="13">
-        <v>3267.4444444444462</v>
-      </c>
-      <c r="AU46" s="14"/>
-      <c r="AX46" s="15"/>
+    <row r="46" spans="1:49">
+      <c r="A46" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B46" s="14">
+        <v>3937.0555555555566</v>
+      </c>
+      <c r="C46" s="14">
+        <v>7832.0555555555547</v>
+      </c>
+      <c r="D46" s="14">
+        <v>4656.8888888888905</v>
+      </c>
+      <c r="E46" s="14">
+        <v>4523.9444444444453</v>
+      </c>
+      <c r="F46" s="14">
+        <v>13110.277777777779</v>
+      </c>
+      <c r="G46" s="14">
+        <v>5433.4444444444443</v>
+      </c>
+      <c r="H46" s="14">
+        <v>8557.3333333333321</v>
+      </c>
+      <c r="I46" s="14">
+        <v>11573.611111111111</v>
+      </c>
+      <c r="J46" s="14">
+        <v>12957.999999999998</v>
+      </c>
+      <c r="K46" s="14">
+        <v>6567.2222222222226</v>
+      </c>
+      <c r="L46" s="14">
+        <v>7999.5</v>
+      </c>
+      <c r="M46" s="14">
+        <v>6943.3333333333321</v>
+      </c>
+      <c r="N46" s="14">
+        <v>5651.1111111111131</v>
+      </c>
+      <c r="O46" s="14">
+        <v>5806.3888888888896</v>
+      </c>
+      <c r="P46" s="14">
+        <v>5341.7222222222208</v>
+      </c>
+      <c r="Q46" s="14">
+        <v>3235.166666666667</v>
+      </c>
+      <c r="R46" s="14">
+        <v>4553.1666666666661</v>
+      </c>
+      <c r="S46" s="14">
+        <v>8121.5</v>
+      </c>
+      <c r="T46" s="14">
+        <v>5921.333333333333</v>
+      </c>
+      <c r="U46" s="14">
+        <v>6714.7777777777765</v>
+      </c>
+      <c r="V46" s="14">
+        <v>6339.5555555555557</v>
+      </c>
+      <c r="W46" s="14">
+        <v>3527.8333333333348</v>
+      </c>
+      <c r="X46" s="14">
+        <v>2780.6111111111104</v>
+      </c>
+      <c r="Y46" s="14">
+        <v>5528.7777777777792</v>
+      </c>
+      <c r="Z46" s="14">
+        <v>6544.9444444444453</v>
+      </c>
+      <c r="AA46" s="14">
+        <v>35968.222222222234</v>
+      </c>
+      <c r="AB46" s="14">
+        <v>38051.722222222226</v>
+      </c>
+      <c r="AC46" s="14">
+        <v>33004.722222222219</v>
+      </c>
+      <c r="AD46" s="14">
+        <v>23122.722222222219</v>
+      </c>
+      <c r="AE46" s="14">
+        <v>11968.388888888889</v>
+      </c>
+      <c r="AF46" s="14">
+        <v>13219.444444444443</v>
+      </c>
+      <c r="AG46" s="14">
+        <v>7910.5</v>
+      </c>
+      <c r="AH46" s="14">
+        <v>12898.111111111108</v>
+      </c>
+      <c r="AI46" s="14">
+        <v>9560.6111111111113</v>
+      </c>
+      <c r="AJ46" s="14">
+        <v>4463.5555555555557</v>
+      </c>
+      <c r="AK46" s="14">
+        <v>2762.5000000000005</v>
+      </c>
+      <c r="AL46" s="14">
+        <v>6815.6111111111122</v>
+      </c>
+      <c r="AM46" s="14">
+        <v>2703.2222222222222</v>
+      </c>
+      <c r="AN46" s="14">
+        <v>5650.8888888888887</v>
+      </c>
+      <c r="AO46" s="14">
+        <v>3349.3333333333339</v>
+      </c>
+      <c r="AP46" s="14">
+        <v>3501.3333333333339</v>
+      </c>
+      <c r="AQ46" s="14">
+        <v>6200.6666666666679</v>
+      </c>
+      <c r="AR46" s="14">
+        <v>6414.8888888888896</v>
+      </c>
+      <c r="AS46" s="14">
+        <v>394897.27777777781</v>
+      </c>
+      <c r="AT46" s="14"/>
+      <c r="AW46" s="15"/>
     </row>
-    <row r="47" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A47" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B47" s="14">
-        <v>3937.0555555555566</v>
-      </c>
-      <c r="C47" s="14">
-        <v>7832.0555555555547</v>
-      </c>
-      <c r="D47" s="14">
-        <v>4656.8888888888905</v>
-      </c>
-      <c r="E47" s="14">
-        <v>4523.9444444444453</v>
-      </c>
-      <c r="F47" s="14">
-        <v>13110.277777777779</v>
-      </c>
-      <c r="G47" s="14">
-        <v>5433.4444444444443</v>
-      </c>
-      <c r="H47" s="14">
-        <v>8557.3333333333321</v>
-      </c>
-      <c r="I47" s="14">
-        <v>11573.611111111111</v>
-      </c>
-      <c r="J47" s="14">
-        <v>12957.999999999998</v>
-      </c>
-      <c r="K47" s="14">
-        <v>6567.2222222222226</v>
-      </c>
-      <c r="L47" s="14">
-        <v>7999.5</v>
-      </c>
-      <c r="M47" s="14">
-        <v>6943.3333333333321</v>
-      </c>
-      <c r="N47" s="14">
-        <v>5651.1111111111131</v>
-      </c>
-      <c r="O47" s="14">
-        <v>5806.3888888888896</v>
-      </c>
-      <c r="P47" s="14">
-        <v>5341.7222222222208</v>
-      </c>
-      <c r="Q47" s="14">
-        <v>3235.166666666667</v>
-      </c>
-      <c r="R47" s="14">
-        <v>4553.1666666666661</v>
-      </c>
-      <c r="S47" s="14">
-        <v>8121.5</v>
-      </c>
-      <c r="T47" s="14">
-        <v>5921.333333333333</v>
-      </c>
-      <c r="U47" s="14">
-        <v>6714.7777777777765</v>
-      </c>
-      <c r="V47" s="14">
-        <v>6339.5555555555557</v>
-      </c>
-      <c r="W47" s="14">
-        <v>3527.8333333333348</v>
-      </c>
-      <c r="X47" s="14">
-        <v>2780.6111111111104</v>
-      </c>
-      <c r="Y47" s="14">
-        <v>5528.7777777777792</v>
-      </c>
-      <c r="Z47" s="14">
-        <v>6544.9444444444453</v>
-      </c>
-      <c r="AA47" s="14">
-        <v>35968.222222222234</v>
-      </c>
-      <c r="AB47" s="14">
-        <v>38051.722222222226</v>
-      </c>
-      <c r="AC47" s="14">
-        <v>33004.722222222219</v>
-      </c>
-      <c r="AD47" s="14">
-        <v>23122.722222222219</v>
-      </c>
-      <c r="AE47" s="14">
-        <v>11968.388888888889</v>
-      </c>
-      <c r="AF47" s="14">
-        <v>13219.444444444443</v>
-      </c>
-      <c r="AG47" s="14">
-        <v>7910.5</v>
-      </c>
-      <c r="AH47" s="14">
-        <v>12898.111111111108</v>
-      </c>
-      <c r="AI47" s="14">
-        <v>9560.6111111111113</v>
-      </c>
-      <c r="AJ47" s="14">
-        <v>4463.5555555555557</v>
-      </c>
-      <c r="AK47" s="14">
-        <v>2762.5000000000005</v>
-      </c>
-      <c r="AL47" s="14">
-        <v>6815.6111111111122</v>
-      </c>
-      <c r="AM47" s="14">
-        <v>2703.2222222222222</v>
-      </c>
-      <c r="AN47" s="14">
-        <v>5650.8888888888887</v>
-      </c>
-      <c r="AO47" s="14">
-        <v>3349.3333333333339</v>
-      </c>
-      <c r="AP47" s="14">
-        <v>3501.3333333333339</v>
-      </c>
-      <c r="AQ47" s="14">
-        <v>6200.6666666666679</v>
-      </c>
-      <c r="AR47" s="14">
-        <v>6414.8888888888896</v>
-      </c>
-      <c r="AS47" s="14">
-        <v>3171.2777777777783</v>
-      </c>
-      <c r="AT47" s="14">
-        <v>394897.27777777781</v>
-      </c>
-      <c r="AU47" s="14"/>
-      <c r="AX47" s="15"/>
+    <row r="47" spans="1:49">
+      <c r="AS47" s="14"/>
+      <c r="AW47" s="15"/>
     </row>
-    <row r="48" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="AT48" s="14"/>
-      <c r="AX48" s="15"/>
+    <row r="48" spans="1:49">
+      <c r="AW48" s="15"/>
     </row>
-    <row r="49" spans="50:50" x14ac:dyDescent="0.2">
-      <c r="AX49" s="15"/>
+    <row r="49" spans="49:49">
+      <c r="AW49" s="15"/>
     </row>
-    <row r="50" spans="50:50" x14ac:dyDescent="0.2">
-      <c r="AX50" s="15"/>
+    <row r="50" spans="49:49">
+      <c r="AW50" s="15"/>
     </row>
-    <row r="51" spans="50:50" x14ac:dyDescent="0.2">
-      <c r="AX51" s="15"/>
+    <row r="51" spans="49:49">
+      <c r="AW51" s="15"/>
     </row>
-    <row r="52" spans="50:50" x14ac:dyDescent="0.2">
-      <c r="AX52" s="15"/>
+    <row r="52" spans="49:49">
+      <c r="AW52" s="15"/>
     </row>
-    <row r="53" spans="50:50" x14ac:dyDescent="0.2">
-      <c r="AX53" s="15"/>
+    <row r="53" spans="49:49">
+      <c r="AW53" s="15"/>
     </row>
-    <row r="54" spans="50:50" x14ac:dyDescent="0.2">
-      <c r="AX54" s="15"/>
+    <row r="54" spans="49:49">
+      <c r="AW54" s="15"/>
     </row>
-    <row r="55" spans="50:50" x14ac:dyDescent="0.2">
-      <c r="AX55" s="15"/>
+    <row r="55" spans="49:49">
+      <c r="AW55" s="15"/>
     </row>
-    <row r="56" spans="50:50" x14ac:dyDescent="0.2">
-      <c r="AX56" s="15"/>
+    <row r="56" spans="49:49">
+      <c r="AW56" s="15"/>
     </row>
-    <row r="57" spans="50:50" x14ac:dyDescent="0.2">
-      <c r="AX57" s="15"/>
+    <row r="57" spans="49:49">
+      <c r="AW57" s="15"/>
     </row>
-    <row r="58" spans="50:50" x14ac:dyDescent="0.2">
-      <c r="AX58" s="15"/>
+    <row r="58" spans="49:49">
+      <c r="AW58" s="15"/>
     </row>
-    <row r="59" spans="50:50" x14ac:dyDescent="0.2">
-      <c r="AX59" s="15"/>
+    <row r="59" spans="49:49">
+      <c r="AW59" s="15"/>
     </row>
-    <row r="60" spans="50:50" x14ac:dyDescent="0.2">
-      <c r="AX60" s="15"/>
+    <row r="60" spans="49:49">
+      <c r="AW60" s="15"/>
     </row>
-    <row r="61" spans="50:50" x14ac:dyDescent="0.2">
-      <c r="AX61" s="15"/>
+    <row r="61" spans="49:49">
+      <c r="AW61" s="15"/>
     </row>
-    <row r="62" spans="50:50" x14ac:dyDescent="0.2">
-      <c r="AX62" s="15"/>
+    <row r="62" spans="49:49">
+      <c r="AW62" s="15"/>
     </row>
-    <row r="63" spans="50:50" x14ac:dyDescent="0.2">
-      <c r="AX63" s="15"/>
-    </row>
-    <row r="64" spans="50:50" x14ac:dyDescent="0.2">
-      <c r="AX64" s="15"/>
+    <row r="63" spans="49:49">
+      <c r="AW63" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="81" fitToWidth="3" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="81" fitToWidth="3" orientation="landscape"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:BE64"/>
@@ -7788,17 +7523,17 @@
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="45" width="7.7109375" style="9" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="8.7109375" style="11" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="9.140625" style="11" collapsed="1"/>
-    <col min="48" max="49" width="9.140625" style="9" collapsed="1"/>
-    <col min="50" max="50" width="8.7109375" style="9" customWidth="1" collapsed="1"/>
-    <col min="51" max="16384" width="9.140625" style="9" collapsed="1"/>
+    <col min="1" max="45" width="7.6640625" style="9" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="8.6640625" style="11" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="8.83203125" style="11" collapsed="1"/>
+    <col min="48" max="49" width="8.83203125" style="9" collapsed="1"/>
+    <col min="50" max="50" width="8.6640625" style="9" customWidth="1" collapsed="1"/>
+    <col min="51" max="16384" width="8.83203125" style="9" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:57" ht="27" customHeight="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -7813,7 +7548,7 @@
         <v>41579</v>
       </c>
     </row>
-    <row r="2" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:57">
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
@@ -7950,7 +7685,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:57">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -8109,7 +7844,7 @@
         <v>0.5936236136527</v>
       </c>
     </row>
-    <row r="4" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:57">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -8268,7 +8003,7 @@
         <v>0.37398903213562623</v>
       </c>
     </row>
-    <row r="5" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:57">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -8416,7 +8151,7 @@
         <v>99406.399999999921</v>
       </c>
     </row>
-    <row r="6" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:57">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -8558,7 +8293,7 @@
       <c r="AU6" s="14"/>
       <c r="AX6" s="12"/>
     </row>
-    <row r="7" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:57">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -8700,7 +8435,7 @@
       <c r="AU7" s="14"/>
       <c r="AX7" s="12"/>
     </row>
-    <row r="8" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:57">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -8842,7 +8577,7 @@
       <c r="AU8" s="14"/>
       <c r="AX8" s="15"/>
     </row>
-    <row r="9" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:57">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -8984,7 +8719,7 @@
       <c r="AU9" s="14"/>
       <c r="AX9" s="15"/>
     </row>
-    <row r="10" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:57">
       <c r="A10" s="1">
         <v>19</v>
       </c>
@@ -9128,7 +8863,7 @@
       <c r="AX10" s="15"/>
       <c r="BD10" s="11"/>
     </row>
-    <row r="11" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:57">
       <c r="A11" s="1">
         <v>12</v>
       </c>
@@ -9294,7 +9029,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:57">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -9470,7 +9205,7 @@
         <v>62992.2</v>
       </c>
     </row>
-    <row r="13" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:57">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -9646,7 +9381,7 @@
         <v>20086.599999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:57">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -9822,7 +9557,7 @@
         <v>35170.400000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:57">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -9998,7 +9733,7 @@
         <v>25537.8</v>
       </c>
     </row>
-    <row r="16" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:57">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -10174,7 +9909,7 @@
         <v>17717.799999999996</v>
       </c>
     </row>
-    <row r="17" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:57">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -10350,7 +10085,7 @@
         <v>31077.8</v>
       </c>
     </row>
-    <row r="18" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:57">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -10526,7 +10261,7 @@
         <v>10811.599999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:57">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -10702,7 +10437,7 @@
         <v>203394.2</v>
       </c>
     </row>
-    <row r="20" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:57">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -10845,7 +10580,7 @@
       <c r="AW20" s="18"/>
       <c r="AX20" s="15"/>
     </row>
-    <row r="21" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:57">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
@@ -11008,7 +10743,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:57">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -11158,7 +10893,7 @@
       <c r="AY22" s="15"/>
       <c r="AZ22" s="15"/>
     </row>
-    <row r="23" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:57">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
@@ -11312,7 +11047,7 @@
       <c r="AZ23" s="15"/>
       <c r="BA23" s="15"/>
     </row>
-    <row r="24" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:57">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -11470,7 +11205,7 @@
       <c r="BA24" s="15"/>
       <c r="BB24" s="15"/>
     </row>
-    <row r="25" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:57">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
@@ -11633,7 +11368,7 @@
       <c r="BC25" s="15"/>
       <c r="BD25" s="14"/>
     </row>
-    <row r="26" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:57">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -11797,7 +11532,7 @@
         <v>3504.1999999999989</v>
       </c>
     </row>
-    <row r="27" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:57">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
@@ -11965,7 +11700,7 @@
         <v>9537.2000000000007</v>
       </c>
     </row>
-    <row r="28" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:57">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -12141,7 +11876,7 @@
         <v>203394.2</v>
       </c>
     </row>
-    <row r="29" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:57">
       <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
@@ -12283,7 +12018,7 @@
       <c r="AU29" s="14"/>
       <c r="AX29" s="15"/>
     </row>
-    <row r="30" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:57">
       <c r="A30" s="1" t="s">
         <v>27</v>
       </c>
@@ -12425,7 +12160,7 @@
       <c r="AU30" s="14"/>
       <c r="AX30" s="15"/>
     </row>
-    <row r="31" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:57">
       <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
@@ -12567,7 +12302,7 @@
       <c r="AU31" s="14"/>
       <c r="AX31" s="15"/>
     </row>
-    <row r="32" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:57">
       <c r="A32" s="1">
         <v>16</v>
       </c>
@@ -12709,7 +12444,7 @@
       <c r="AU32" s="14"/>
       <c r="AX32" s="15"/>
     </row>
-    <row r="33" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:50">
       <c r="A33" s="1">
         <v>24</v>
       </c>
@@ -12851,7 +12586,7 @@
       <c r="AU33" s="14"/>
       <c r="AX33" s="15"/>
     </row>
-    <row r="34" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:50">
       <c r="A34" s="1" t="s">
         <v>29</v>
       </c>
@@ -12993,7 +12728,7 @@
       <c r="AU34" s="14"/>
       <c r="AX34" s="15"/>
     </row>
-    <row r="35" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:50">
       <c r="A35" s="1" t="s">
         <v>30</v>
       </c>
@@ -13135,7 +12870,7 @@
       <c r="AU35" s="14"/>
       <c r="AX35" s="15"/>
     </row>
-    <row r="36" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:50">
       <c r="A36" s="1" t="s">
         <v>31</v>
       </c>
@@ -13277,7 +13012,7 @@
       <c r="AU36" s="14"/>
       <c r="AX36" s="15"/>
     </row>
-    <row r="37" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:50">
       <c r="A37" s="1" t="s">
         <v>32</v>
       </c>
@@ -13419,7 +13154,7 @@
       <c r="AU37" s="14"/>
       <c r="AX37" s="15"/>
     </row>
-    <row r="38" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:50">
       <c r="A38" s="1" t="s">
         <v>33</v>
       </c>
@@ -13561,7 +13296,7 @@
       <c r="AU38" s="14"/>
       <c r="AX38" s="15"/>
     </row>
-    <row r="39" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:50">
       <c r="A39" s="1" t="s">
         <v>34</v>
       </c>
@@ -13703,7 +13438,7 @@
       <c r="AU39" s="14"/>
       <c r="AX39" s="15"/>
     </row>
-    <row r="40" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:50">
       <c r="A40" s="1" t="s">
         <v>35</v>
       </c>
@@ -13845,7 +13580,7 @@
       <c r="AU40" s="14"/>
       <c r="AX40" s="15"/>
     </row>
-    <row r="41" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:50">
       <c r="A41" s="1" t="s">
         <v>36</v>
       </c>
@@ -13987,7 +13722,7 @@
       <c r="AU41" s="14"/>
       <c r="AX41" s="15"/>
     </row>
-    <row r="42" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:50">
       <c r="A42" s="1" t="s">
         <v>53</v>
       </c>
@@ -14129,7 +13864,7 @@
       <c r="AU42" s="14"/>
       <c r="AX42" s="15"/>
     </row>
-    <row r="43" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:50">
       <c r="A43" s="1" t="s">
         <v>54</v>
       </c>
@@ -14271,7 +14006,7 @@
       <c r="AU43" s="14"/>
       <c r="AX43" s="15"/>
     </row>
-    <row r="44" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:50">
       <c r="A44" s="1" t="s">
         <v>55</v>
       </c>
@@ -14413,7 +14148,7 @@
       <c r="AU44" s="14"/>
       <c r="AX44" s="15"/>
     </row>
-    <row r="45" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:50">
       <c r="A45" s="1" t="s">
         <v>56</v>
       </c>
@@ -14555,7 +14290,7 @@
       <c r="AU45" s="14"/>
       <c r="AX45" s="15"/>
     </row>
-    <row r="46" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:50">
       <c r="A46" s="1" t="s">
         <v>62</v>
       </c>
@@ -14697,7 +14432,7 @@
       <c r="AU46" s="14"/>
       <c r="AX46" s="15"/>
     </row>
-    <row r="47" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:50">
       <c r="A47" s="11" t="s">
         <v>49</v>
       </c>
@@ -14839,69 +14574,74 @@
       <c r="AU47" s="14"/>
       <c r="AX47" s="15"/>
     </row>
-    <row r="48" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:50">
       <c r="AT48" s="14"/>
       <c r="AX48" s="15"/>
     </row>
-    <row r="49" spans="50:50" x14ac:dyDescent="0.2">
+    <row r="49" spans="50:50">
       <c r="AX49" s="15"/>
     </row>
-    <row r="50" spans="50:50" x14ac:dyDescent="0.2">
+    <row r="50" spans="50:50">
       <c r="AX50" s="15"/>
     </row>
-    <row r="51" spans="50:50" x14ac:dyDescent="0.2">
+    <row r="51" spans="50:50">
       <c r="AX51" s="15"/>
     </row>
-    <row r="52" spans="50:50" x14ac:dyDescent="0.2">
+    <row r="52" spans="50:50">
       <c r="AX52" s="15"/>
     </row>
-    <row r="53" spans="50:50" x14ac:dyDescent="0.2">
+    <row r="53" spans="50:50">
       <c r="AX53" s="15"/>
     </row>
-    <row r="54" spans="50:50" x14ac:dyDescent="0.2">
+    <row r="54" spans="50:50">
       <c r="AX54" s="15"/>
     </row>
-    <row r="55" spans="50:50" x14ac:dyDescent="0.2">
+    <row r="55" spans="50:50">
       <c r="AX55" s="15"/>
     </row>
-    <row r="56" spans="50:50" x14ac:dyDescent="0.2">
+    <row r="56" spans="50:50">
       <c r="AX56" s="15"/>
     </row>
-    <row r="57" spans="50:50" x14ac:dyDescent="0.2">
+    <row r="57" spans="50:50">
       <c r="AX57" s="15"/>
     </row>
-    <row r="58" spans="50:50" x14ac:dyDescent="0.2">
+    <row r="58" spans="50:50">
       <c r="AX58" s="15"/>
     </row>
-    <row r="59" spans="50:50" x14ac:dyDescent="0.2">
+    <row r="59" spans="50:50">
       <c r="AX59" s="15"/>
     </row>
-    <row r="60" spans="50:50" x14ac:dyDescent="0.2">
+    <row r="60" spans="50:50">
       <c r="AX60" s="15"/>
     </row>
-    <row r="61" spans="50:50" x14ac:dyDescent="0.2">
+    <row r="61" spans="50:50">
       <c r="AX61" s="15"/>
     </row>
-    <row r="62" spans="50:50" x14ac:dyDescent="0.2">
+    <row r="62" spans="50:50">
       <c r="AX62" s="15"/>
     </row>
-    <row r="63" spans="50:50" x14ac:dyDescent="0.2">
+    <row r="63" spans="50:50">
       <c r="AX63" s="15"/>
     </row>
-    <row r="64" spans="50:50" x14ac:dyDescent="0.2">
+    <row r="64" spans="50:50">
       <c r="AX64" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="72" fitToWidth="2" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="72" fitToWidth="2" orientation="landscape"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:BE64"/>
@@ -14914,17 +14654,17 @@
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="45" width="7.7109375" style="9" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="8.7109375" style="11" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="9.140625" style="11" collapsed="1"/>
-    <col min="48" max="49" width="9.140625" style="9" collapsed="1"/>
-    <col min="50" max="50" width="8.7109375" style="9" customWidth="1" collapsed="1"/>
-    <col min="51" max="16384" width="9.140625" style="9" collapsed="1"/>
+    <col min="1" max="45" width="7.6640625" style="9" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="8.6640625" style="11" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="8.83203125" style="11" collapsed="1"/>
+    <col min="48" max="49" width="8.83203125" style="9" collapsed="1"/>
+    <col min="50" max="50" width="8.6640625" style="9" customWidth="1" collapsed="1"/>
+    <col min="51" max="16384" width="8.83203125" style="9" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:57" ht="26.25" customHeight="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -14939,7 +14679,7 @@
         <v>41579</v>
       </c>
     </row>
-    <row r="2" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:57">
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
@@ -15076,7 +14816,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:57">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -15235,7 +14975,7 @@
         <v>0.55450943069735248</v>
       </c>
     </row>
-    <row r="4" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:57">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -15394,7 +15134,7 @@
         <v>0.40469631424121821</v>
       </c>
     </row>
-    <row r="5" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:57">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -15542,7 +15282,7 @@
         <v>65694.25</v>
       </c>
     </row>
-    <row r="6" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:57">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -15684,7 +15424,7 @@
       <c r="AU6" s="14"/>
       <c r="AX6" s="12"/>
     </row>
-    <row r="7" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:57">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -15826,7 +15566,7 @@
       <c r="AU7" s="14"/>
       <c r="AX7" s="12"/>
     </row>
-    <row r="8" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:57">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -15968,7 +15708,7 @@
       <c r="AU8" s="14"/>
       <c r="AX8" s="15"/>
     </row>
-    <row r="9" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:57">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -16110,7 +15850,7 @@
       <c r="AU9" s="14"/>
       <c r="AX9" s="15"/>
     </row>
-    <row r="10" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:57">
       <c r="A10" s="1">
         <v>19</v>
       </c>
@@ -16254,7 +15994,7 @@
       <c r="AX10" s="15"/>
       <c r="BD10" s="11"/>
     </row>
-    <row r="11" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:57">
       <c r="A11" s="1">
         <v>12</v>
       </c>
@@ -16420,7 +16160,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:57">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -16596,7 +16336,7 @@
         <v>40425</v>
       </c>
     </row>
-    <row r="13" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:57">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -16772,7 +16512,7 @@
         <v>14981.5</v>
       </c>
     </row>
-    <row r="14" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:57">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -16948,7 +16688,7 @@
         <v>24376.5</v>
       </c>
     </row>
-    <row r="15" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:57">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -17124,7 +16864,7 @@
         <v>16023.75</v>
       </c>
     </row>
-    <row r="16" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:57">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -17300,7 +17040,7 @@
         <v>12482.5</v>
       </c>
     </row>
-    <row r="17" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:57">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -17476,7 +17216,7 @@
         <v>27044.5</v>
       </c>
     </row>
-    <row r="18" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:57">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -17652,7 +17392,7 @@
         <v>9141.25</v>
       </c>
     </row>
-    <row r="19" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:57">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -17828,7 +17568,7 @@
         <v>144475</v>
       </c>
     </row>
-    <row r="20" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:57">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -17971,7 +17711,7 @@
       <c r="AW20" s="18"/>
       <c r="AX20" s="15"/>
     </row>
-    <row r="21" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:57">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
@@ -18134,7 +17874,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:57">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -18284,7 +18024,7 @@
       <c r="AY22" s="15"/>
       <c r="AZ22" s="15"/>
     </row>
-    <row r="23" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:57">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
@@ -18438,7 +18178,7 @@
       <c r="AZ23" s="15"/>
       <c r="BA23" s="15"/>
     </row>
-    <row r="24" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:57">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -18596,7 +18336,7 @@
       <c r="BA24" s="15"/>
       <c r="BB24" s="15"/>
     </row>
-    <row r="25" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:57">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
@@ -18759,7 +18499,7 @@
       <c r="BC25" s="15"/>
       <c r="BD25" s="14"/>
     </row>
-    <row r="26" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:57">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -18923,7 +18663,7 @@
         <v>2381.75</v>
       </c>
     </row>
-    <row r="27" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:57">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
@@ -19091,7 +18831,7 @@
         <v>10989.5</v>
       </c>
     </row>
-    <row r="28" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:57">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -19267,7 +19007,7 @@
         <v>144475</v>
       </c>
     </row>
-    <row r="29" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:57">
       <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
@@ -19409,7 +19149,7 @@
       <c r="AU29" s="14"/>
       <c r="AX29" s="15"/>
     </row>
-    <row r="30" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:57">
       <c r="A30" s="1" t="s">
         <v>27</v>
       </c>
@@ -19551,7 +19291,7 @@
       <c r="AU30" s="14"/>
       <c r="AX30" s="15"/>
     </row>
-    <row r="31" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:57">
       <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
@@ -19693,7 +19433,7 @@
       <c r="AU31" s="14"/>
       <c r="AX31" s="15"/>
     </row>
-    <row r="32" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:57">
       <c r="A32" s="1">
         <v>16</v>
       </c>
@@ -19835,7 +19575,7 @@
       <c r="AU32" s="14"/>
       <c r="AX32" s="15"/>
     </row>
-    <row r="33" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:50">
       <c r="A33" s="1">
         <v>24</v>
       </c>
@@ -19977,7 +19717,7 @@
       <c r="AU33" s="14"/>
       <c r="AX33" s="15"/>
     </row>
-    <row r="34" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:50">
       <c r="A34" s="1" t="s">
         <v>29</v>
       </c>
@@ -20119,7 +19859,7 @@
       <c r="AU34" s="14"/>
       <c r="AX34" s="15"/>
     </row>
-    <row r="35" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:50">
       <c r="A35" s="1" t="s">
         <v>30</v>
       </c>
@@ -20261,7 +20001,7 @@
       <c r="AU35" s="14"/>
       <c r="AX35" s="15"/>
     </row>
-    <row r="36" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:50">
       <c r="A36" s="1" t="s">
         <v>31</v>
       </c>
@@ -20403,7 +20143,7 @@
       <c r="AU36" s="14"/>
       <c r="AX36" s="15"/>
     </row>
-    <row r="37" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:50">
       <c r="A37" s="1" t="s">
         <v>32</v>
       </c>
@@ -20545,7 +20285,7 @@
       <c r="AU37" s="14"/>
       <c r="AX37" s="15"/>
     </row>
-    <row r="38" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:50">
       <c r="A38" s="1" t="s">
         <v>33</v>
       </c>
@@ -20687,7 +20427,7 @@
       <c r="AU38" s="14"/>
       <c r="AX38" s="15"/>
     </row>
-    <row r="39" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:50">
       <c r="A39" s="1" t="s">
         <v>34</v>
       </c>
@@ -20829,7 +20569,7 @@
       <c r="AU39" s="14"/>
       <c r="AX39" s="15"/>
     </row>
-    <row r="40" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:50">
       <c r="A40" s="1" t="s">
         <v>35</v>
       </c>
@@ -20971,7 +20711,7 @@
       <c r="AU40" s="14"/>
       <c r="AX40" s="15"/>
     </row>
-    <row r="41" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:50">
       <c r="A41" s="1" t="s">
         <v>36</v>
       </c>
@@ -21113,7 +20853,7 @@
       <c r="AU41" s="14"/>
       <c r="AX41" s="15"/>
     </row>
-    <row r="42" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:50">
       <c r="A42" s="1" t="s">
         <v>53</v>
       </c>
@@ -21255,7 +20995,7 @@
       <c r="AU42" s="14"/>
       <c r="AX42" s="15"/>
     </row>
-    <row r="43" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:50">
       <c r="A43" s="1" t="s">
         <v>54</v>
       </c>
@@ -21397,7 +21137,7 @@
       <c r="AU43" s="14"/>
       <c r="AX43" s="15"/>
     </row>
-    <row r="44" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:50">
       <c r="A44" s="1" t="s">
         <v>55</v>
       </c>
@@ -21539,7 +21279,7 @@
       <c r="AU44" s="14"/>
       <c r="AX44" s="15"/>
     </row>
-    <row r="45" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:50">
       <c r="A45" s="1" t="s">
         <v>56</v>
       </c>
@@ -21681,7 +21421,7 @@
       <c r="AU45" s="14"/>
       <c r="AX45" s="15"/>
     </row>
-    <row r="46" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:50">
       <c r="A46" s="1" t="s">
         <v>62</v>
       </c>
@@ -21823,7 +21563,7 @@
       <c r="AU46" s="14"/>
       <c r="AX46" s="15"/>
     </row>
-    <row r="47" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:50">
       <c r="A47" s="11" t="s">
         <v>49</v>
       </c>
@@ -21965,63 +21705,68 @@
       <c r="AU47" s="14"/>
       <c r="AX47" s="15"/>
     </row>
-    <row r="48" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:50">
       <c r="AT48" s="14"/>
       <c r="AX48" s="15"/>
     </row>
-    <row r="49" spans="50:50" x14ac:dyDescent="0.2">
+    <row r="49" spans="50:50">
       <c r="AX49" s="15"/>
     </row>
-    <row r="50" spans="50:50" x14ac:dyDescent="0.2">
+    <row r="50" spans="50:50">
       <c r="AX50" s="15"/>
     </row>
-    <row r="51" spans="50:50" x14ac:dyDescent="0.2">
+    <row r="51" spans="50:50">
       <c r="AX51" s="15"/>
     </row>
-    <row r="52" spans="50:50" x14ac:dyDescent="0.2">
+    <row r="52" spans="50:50">
       <c r="AX52" s="15"/>
     </row>
-    <row r="53" spans="50:50" x14ac:dyDescent="0.2">
+    <row r="53" spans="50:50">
       <c r="AX53" s="15"/>
     </row>
-    <row r="54" spans="50:50" x14ac:dyDescent="0.2">
+    <row r="54" spans="50:50">
       <c r="AX54" s="15"/>
     </row>
-    <row r="55" spans="50:50" x14ac:dyDescent="0.2">
+    <row r="55" spans="50:50">
       <c r="AX55" s="15"/>
     </row>
-    <row r="56" spans="50:50" x14ac:dyDescent="0.2">
+    <row r="56" spans="50:50">
       <c r="AX56" s="15"/>
     </row>
-    <row r="57" spans="50:50" x14ac:dyDescent="0.2">
+    <row r="57" spans="50:50">
       <c r="AX57" s="15"/>
     </row>
-    <row r="58" spans="50:50" x14ac:dyDescent="0.2">
+    <row r="58" spans="50:50">
       <c r="AX58" s="15"/>
     </row>
-    <row r="59" spans="50:50" x14ac:dyDescent="0.2">
+    <row r="59" spans="50:50">
       <c r="AX59" s="15"/>
     </row>
-    <row r="60" spans="50:50" x14ac:dyDescent="0.2">
+    <row r="60" spans="50:50">
       <c r="AX60" s="15"/>
     </row>
-    <row r="61" spans="50:50" x14ac:dyDescent="0.2">
+    <row r="61" spans="50:50">
       <c r="AX61" s="15"/>
     </row>
-    <row r="62" spans="50:50" x14ac:dyDescent="0.2">
+    <row r="62" spans="50:50">
       <c r="AX62" s="15"/>
     </row>
-    <row r="63" spans="50:50" x14ac:dyDescent="0.2">
+    <row r="63" spans="50:50">
       <c r="AX63" s="15"/>
     </row>
-    <row r="64" spans="50:50" x14ac:dyDescent="0.2">
+    <row r="64" spans="50:50">
       <c r="AX64" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="72" fitToWidth="2" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="72" fitToWidth="2" orientation="landscape"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -22033,12 +21778,12 @@
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="10" width="8.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="10" width="8.1640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" s="2" t="s">
         <v>63</v>
       </c>
@@ -22048,12 +21793,12 @@
         <v>41579</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="B4" s="1" t="s">
         <v>25</v>
       </c>
@@ -22082,7 +21827,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -22114,7 +21859,7 @@
         <v>2750.3333333333335</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
@@ -22146,7 +21891,7 @@
         <v>4058.1111111111113</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
@@ -22178,7 +21923,7 @@
         <v>3005.1666666666665</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
@@ -22210,7 +21955,7 @@
         <v>1964.6111111111109</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
         <v>16</v>
       </c>
@@ -22242,7 +21987,7 @@
         <v>1969.8333333333335</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
         <v>24</v>
       </c>
@@ -22274,7 +22019,7 @@
         <v>2889.2777777777783</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
@@ -22306,7 +22051,7 @@
         <v>2412.2777777777778</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10">
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
@@ -22338,7 +22083,7 @@
         <v>5050</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" s="3" customFormat="1">
       <c r="A13" s="3" t="s">
         <v>49</v>
       </c>
@@ -22370,7 +22115,7 @@
         <v>24100</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -22381,7 +22126,7 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -22395,7 +22140,7 @@
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10">
       <c r="B16" s="6" t="s">
         <v>25</v>
       </c>
@@ -22424,7 +22169,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10">
       <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
@@ -22456,7 +22201,7 @@
         <v>742.2</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10">
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
@@ -22488,7 +22233,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10">
       <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
@@ -22520,7 +22265,7 @@
         <v>2330.1999999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10">
       <c r="A20" s="1" t="s">
         <v>28</v>
       </c>
@@ -22552,7 +22297,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10">
       <c r="A21" s="1">
         <v>16</v>
       </c>
@@ -22584,7 +22329,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10">
       <c r="A22" s="1">
         <v>24</v>
       </c>
@@ -22616,7 +22361,7 @@
         <v>1375.2</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10">
       <c r="A23" s="1" t="s">
         <v>29</v>
       </c>
@@ -22648,7 +22393,7 @@
         <v>956.6</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -22680,7 +22425,7 @@
         <v>2364.1999999999998</v>
       </c>
     </row>
-    <row r="25" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" s="3" customFormat="1">
       <c r="A25" s="3" t="s">
         <v>49</v>
       </c>
@@ -22712,7 +22457,7 @@
         <v>10861</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10">
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -22723,7 +22468,7 @@
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10">
       <c r="A27" t="s">
         <v>52</v>
       </c>
@@ -22737,7 +22482,7 @@
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10">
       <c r="B28" s="6" t="s">
         <v>25</v>
       </c>
@@ -22766,7 +22511,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10">
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
@@ -22798,7 +22543,7 @@
         <v>491.25</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10">
       <c r="A30" s="1" t="s">
         <v>26</v>
       </c>
@@ -22830,7 +22575,7 @@
         <v>790.5</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10">
       <c r="A31" s="1" t="s">
         <v>27</v>
       </c>
@@ -22862,7 +22607,7 @@
         <v>1585</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10">
       <c r="A32" s="1" t="s">
         <v>28</v>
       </c>
@@ -22894,7 +22639,7 @@
         <v>616.25</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10">
       <c r="A33" s="1">
         <v>16</v>
       </c>
@@ -22926,7 +22671,7 @@
         <v>841.25</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10">
       <c r="A34" s="1">
         <v>24</v>
       </c>
@@ -22958,7 +22703,7 @@
         <v>1020.25</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10">
       <c r="A35" s="1" t="s">
         <v>29</v>
       </c>
@@ -22990,7 +22735,7 @@
         <v>730.5</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10">
       <c r="A36" s="1" t="s">
         <v>30</v>
       </c>
@@ -23022,7 +22767,7 @@
         <v>1838</v>
       </c>
     </row>
-    <row r="37" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" s="3" customFormat="1">
       <c r="A37" s="3" t="s">
         <v>49</v>
       </c>
@@ -23057,7 +22802,12 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>